<commit_message>
Draft comming along. Added migration section and Figure to methods
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HCN-by-Alleles" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="All simulations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -145,13 +146,195 @@
   </si>
   <si>
     <t>Drift (Case 1, see text)</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Drift controlled by</t>
+  </si>
+  <si>
+    <t>Parameters controlling drift</t>
+  </si>
+  <si>
+    <t>Migration rates</t>
+  </si>
+  <si>
+    <t>Total number of simulations</t>
+  </si>
+  <si>
+    <t>0; 0.001; 0.0025; 0.005; 0.01; 0.02; 0.035; 0.05; 0.1; 0.2; 0.35; 0.5</t>
+  </si>
+  <si>
+    <t>0; 0.01; 0.05</t>
+  </si>
+  <si>
+    <t>Colonization</t>
+  </si>
+  <si>
+    <t>None. All patches occupied from start</t>
+  </si>
+  <si>
+    <t>Rural to Urban</t>
+  </si>
+  <si>
+    <t>Serial founder events</t>
+  </si>
+  <si>
+    <t>Max K = 1000 (Rural); Min K = 10 (Urban)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Selection coefficient</t>
+  </si>
+  <si>
+    <t>Initial allele frequencies</t>
+  </si>
+  <si>
+    <t>pA = 0.5; pB = 0.5</t>
+  </si>
+  <si>
+    <t>0; 0.001; 0.0025; 0.005; 0.0075; 0.01; 0.025; 0.05; 0.1; 0.2</t>
+  </si>
+  <si>
+    <t>Mechanisms explored</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frequencies crossed factorially:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pA = 0.1; 0.5; 0.9. pB = 0.1; 0.5; 0.9.</t>
+    </r>
+  </si>
+  <si>
+    <t>Drift and migration</t>
+  </si>
+  <si>
+    <t>Drift and migration with allele frequency variation</t>
+  </si>
+  <si>
+    <t>Selection and migration</t>
+  </si>
+  <si>
+    <t>None. All population with contstant K = 1000</t>
+  </si>
+  <si>
+    <t>Selection, migration and drift</t>
+  </si>
+  <si>
+    <t>3 from above depending on inflection point if results (e.g. 0; 0.005, 0.01)</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Re-run</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Max K = 1000 (Urban); Min K = 10 (Rural)</t>
+  </si>
+  <si>
+    <t>Spatial gradient in K from Rural to Urban</t>
+  </si>
+  <si>
+    <t>Spatial gradient in K from Urban to Rural</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Founder proportion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">           0.01; 0.02; 0.035; 0.05; 0.075; 0.1; 0.2; 0.5; 0.75; 1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Founder proportion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                  0.01; 0.2; 1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Founder proportion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                 0.01; 0.2; 1.0</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,6 +372,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -204,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -304,8 +508,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -315,8 +650,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -370,19 +709,449 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -536,18 +1305,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
   <autoFilter ref="A1:C5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="CYP79D15" dataDxfId="2"/>
-    <tableColumn id="2" name="Li" dataDxfId="1"/>
-    <tableColumn id="3" name="HCN" dataDxfId="0"/>
+    <tableColumn id="1" name="CYP79D15" dataDxfId="16"/>
+    <tableColumn id="2" name="Li" dataDxfId="15"/>
+    <tableColumn id="3" name="HCN" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:I8">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Case" dataDxfId="9"/>
+    <tableColumn id="2" name="Mechanisms explored" dataDxfId="8"/>
+    <tableColumn id="3" name="Colonization" dataDxfId="7"/>
+    <tableColumn id="4" name="Drift controlled by" dataDxfId="6"/>
+    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="5"/>
+    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="4"/>
+    <tableColumn id="7" name="Selection coefficient" dataDxfId="3"/>
+    <tableColumn id="8" name="Migration rates" dataDxfId="2"/>
+    <tableColumn id="9" name="Total number of simulations" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -892,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1046,4 +1843,287 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="19"/>
+    <col min="2" max="2" width="21.83203125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="19" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="27" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="49" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="35">
+        <v>12</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="24">
+        <v>30</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="24">
+        <v>27</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="24">
+        <f>27*3</f>
+        <v>81</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="26">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="28">
+        <v>30</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A7" s="26">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="28">
+        <v>27</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="29">
+        <v>7</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="31">
+        <v>9</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added selection function figure
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-31920" yWindow="3260" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HCN-by-Alleles" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -328,6 +328,12 @@
       </rPr>
       <t xml:space="preserve">                 0.01; 0.2; 1.0</t>
     </r>
+  </si>
+  <si>
+    <t>Urban to Rural</t>
+  </si>
+  <si>
+    <t>Running</t>
   </si>
 </sst>
 </file>
@@ -787,30 +793,6 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1087,6 +1069,53 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1127,29 +1156,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1321,8 +1327,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A1:I8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I9">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1334,15 +1340,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Case" dataDxfId="9"/>
-    <tableColumn id="2" name="Mechanisms explored" dataDxfId="8"/>
-    <tableColumn id="3" name="Colonization" dataDxfId="7"/>
-    <tableColumn id="4" name="Drift controlled by" dataDxfId="6"/>
-    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="5"/>
-    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="4"/>
-    <tableColumn id="7" name="Selection coefficient" dataDxfId="3"/>
-    <tableColumn id="8" name="Migration rates" dataDxfId="2"/>
-    <tableColumn id="9" name="Total number of simulations" dataDxfId="1"/>
+    <tableColumn id="1" name="Case" dataDxfId="8"/>
+    <tableColumn id="2" name="Mechanisms explored" dataDxfId="7"/>
+    <tableColumn id="3" name="Colonization" dataDxfId="6"/>
+    <tableColumn id="4" name="Drift controlled by" dataDxfId="5"/>
+    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="4"/>
+    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="3"/>
+    <tableColumn id="7" name="Selection coefficient" dataDxfId="2"/>
+    <tableColumn id="8" name="Migration rates" dataDxfId="1"/>
+    <tableColumn id="9" name="Total number of simulations" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1847,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1861,9 +1867,9 @@
     <col min="4" max="4" width="20.5" style="19" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" style="19" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="20" style="19" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="27" style="19" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1988,7 +1994,7 @@
         <v>27</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -2053,7 +2059,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -2117,6 +2123,38 @@
         <v>9</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" s="29">
+        <v>8</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="31">
+        <v>27</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added parameters and simulated cases table to draft. Finished writing draft of methods
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -52,15 +52,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Maximum migration rate (m)</t>
-  </si>
-  <si>
-    <t>Maximum carrying capacity (Kmax)</t>
-  </si>
-  <si>
-    <t>Minimum carrying capacity (Kmin)</t>
-  </si>
-  <si>
     <t>Number of rows</t>
   </si>
   <si>
@@ -76,27 +67,9 @@
     <t>Maximum selection coefficient (smax)</t>
   </si>
   <si>
-    <t>Frequency of dominant CYP79D15 (pA)</t>
-  </si>
-  <si>
-    <t>Frequency of dominant Li (pB)</t>
-  </si>
-  <si>
     <t>Number of generations</t>
   </si>
   <si>
-    <t>Number of simulations</t>
-  </si>
-  <si>
-    <t>Determines the maximum proportion of alleles (CYP79D15 and Li) exchanged between any two populations. The actual proportion depends on the distance between populations (Equation X)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Determines the carrying capacity of the largest habitat patch on the landscape. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Determines the carrying capacity of the smallest habitat patch on the landscape. </t>
-  </si>
-  <si>
     <t>Intrinsic rate of population increase</t>
   </si>
   <si>
@@ -109,24 +82,9 @@
     <t xml:space="preserve">Proportion of alleles sampled when founding a new populations. Lower proportions results in stronger effects of drift. </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum probability that a new population is created. Actual probability depends on the populations size such that larger populations have a greater probability of creating new ones. Values is fixed at 1.0 so that populations at carrying capacity are guarenteed to found new populations. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum strength of selection acting on cyanogenic or acyanogenic genotypes. Actual strength of selection depends on position in the landscape matrix. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial frequency of the dominant allele at the CYP79D15 locus. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial frequency of the dominant allele at the Li locus. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Intrinsic growth rate parameter used in logistic equation of population growth. Fixed at 1.5. </t>
   </si>
   <si>
-    <t>Number of simulation to run. Fixed at 1000.</t>
-  </si>
-  <si>
     <t>Number of generations to run simulations once all patched on the landscape have been colonized with populations. Fixed at 500</t>
   </si>
   <si>
@@ -142,15 +100,6 @@
     <t>Within-population dynamics</t>
   </si>
   <si>
-    <t>Drift (Case 2, see text)</t>
-  </si>
-  <si>
-    <t>Drift (Case 1, see text)</t>
-  </si>
-  <si>
-    <t>Case</t>
-  </si>
-  <si>
     <t>Drift controlled by</t>
   </si>
   <si>
@@ -172,9 +121,6 @@
     <t>Colonization</t>
   </si>
   <si>
-    <t>None. All patches occupied from start</t>
-  </si>
-  <si>
     <t>Rural to Urban</t>
   </si>
   <si>
@@ -200,6 +146,217 @@
   </si>
   <si>
     <t>Mechanisms explored</t>
+  </si>
+  <si>
+    <t>Drift and migration</t>
+  </si>
+  <si>
+    <t>Drift and migration with allele frequency variation</t>
+  </si>
+  <si>
+    <t>Selection and migration</t>
+  </si>
+  <si>
+    <t>None. All population with contstant K = 1000</t>
+  </si>
+  <si>
+    <t>Selection, migration and drift</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Re-run</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Max K = 1000 (Urban); Min K = 10 (Rural)</t>
+  </si>
+  <si>
+    <t>Spatial gradient in K from Rural to Urban</t>
+  </si>
+  <si>
+    <t>Spatial gradient in K from Urban to Rural</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Founder proportion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">           0.01; 0.02; 0.035; 0.05; 0.075; 0.1; 0.2; 0.5; 0.75; 1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Founder proportion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                  0.01; 0.2; 1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Founder proportion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                 0.01; 0.2; 1.0</t>
+    </r>
+  </si>
+  <si>
+    <t>Urban to Rural</t>
+  </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>Determines the maximum proportion of alleles (CYP79D15 and Li) exchanged between any two populations. The actual proportion depends on the distance between populations (see text)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determines the carrying capacity of the largest habitat patch on the landscape (rural-most or urban-most population). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determines the carrying capacity of the smallest habitat patch on the landscape (rural-most or urban-most population). </t>
+  </si>
+  <si>
+    <t>Drift (scenario 2, see text)</t>
+  </si>
+  <si>
+    <t>Drift (scenario 1, see text)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum strength of selection acting on cyanogenic or acyanogenic genotypes. Actual strength of selection depends on a population's position in the landscape matrix. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency of dominant CYP79D15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency of dominant Li </t>
+  </si>
+  <si>
+    <t>Minimum carrying capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum carrying capacity </t>
+  </si>
+  <si>
+    <t>Maximum migration rate</t>
+  </si>
+  <si>
+    <t>Number of iterations</t>
+  </si>
+  <si>
+    <t>Number of iterations to run to run for each simulated scenario (see table 3). Fixed at 1000.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initial frequency of the dominant allele at the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CYP79D15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> locus. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initial frequency of the dominant allele at the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Li</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> locus. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum probability that a new population is created. Actual probability depends on the populations size such that larger populations have a greater probability of creating new ones. Value is fixed at 1.0 so that populations at carrying capacity are guaranteed to found new populations. </t>
+  </si>
+  <si>
+    <t>1 (modified)</t>
+  </si>
+  <si>
+    <t>2 (modified)</t>
+  </si>
+  <si>
+    <t>None.</t>
   </si>
   <si>
     <r>
@@ -221,56 +378,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> pA = 0.1; 0.5; 0.9. pB = 0.1; 0.5; 0.9.</t>
+      <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>Drift and migration</t>
-  </si>
-  <si>
-    <t>Drift and migration with allele frequency variation</t>
-  </si>
-  <si>
-    <t>Selection and migration</t>
-  </si>
-  <si>
-    <t>None. All population with contstant K = 1000</t>
-  </si>
-  <si>
-    <t>Selection, migration and drift</t>
-  </si>
-  <si>
-    <t>3 from above depending on inflection point if results (e.g. 0; 0.005, 0.01)</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Re-run</t>
-  </si>
-  <si>
-    <t>Not done</t>
-  </si>
-  <si>
-    <t>Max K = 1000 (Urban); Min K = 10 (Rural)</t>
-  </si>
-  <si>
-    <t>Spatial gradient in K from Rural to Urban</t>
-  </si>
-  <si>
-    <t>Spatial gradient in K from Urban to Rural</t>
-  </si>
-  <si>
     <r>
       <rPr>
-        <b/>
+        <i/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Founder proportion:</t>
+      <t>CYP79D15</t>
     </r>
     <r>
       <rPr>
@@ -280,20 +399,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">           0.01; 0.02; 0.035; 0.05; 0.075; 0.1; 0.2; 0.5; 0.75; 1.0</t>
+      <t xml:space="preserve"> = 0.1; 0.5; 0.9. </t>
     </r>
-  </si>
-  <si>
     <r>
       <rPr>
-        <b/>
+        <i/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Founder proportion:</t>
+      <t>Li</t>
     </r>
     <r>
       <rPr>
@@ -303,44 +420,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                  0.01; 0.2; 1.0</t>
+      <t xml:space="preserve"> = 0.1; 0.5; 0.9.</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Founder proportion:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                 0.01; 0.2; 1.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Urban to Rural</t>
-  </si>
-  <si>
-    <t>Running</t>
+    <t xml:space="preserve">3 from above </t>
+  </si>
+  <si>
+    <t>Drift scenario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -399,8 +493,24 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +520,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,7 +762,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -660,8 +776,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -775,23 +907,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1311,23 +1471,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="A1:C5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="CYP79D15" dataDxfId="16"/>
-    <tableColumn id="2" name="Li" dataDxfId="15"/>
-    <tableColumn id="3" name="HCN" dataDxfId="14"/>
+    <tableColumn id="1" name="CYP79D15" dataDxfId="19"/>
+    <tableColumn id="2" name="Li" dataDxfId="18"/>
+    <tableColumn id="3" name="HCN" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C14" totalsRowShown="0">
+  <autoFilter ref="A1:C14">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Parameter" dataDxfId="2"/>
+    <tableColumn id="2" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" name="Mechanism controlled" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:I9">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1340,15 +1516,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Case" dataDxfId="8"/>
-    <tableColumn id="2" name="Mechanisms explored" dataDxfId="7"/>
-    <tableColumn id="3" name="Colonization" dataDxfId="6"/>
-    <tableColumn id="4" name="Drift controlled by" dataDxfId="5"/>
-    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="4"/>
-    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="3"/>
-    <tableColumn id="7" name="Selection coefficient" dataDxfId="2"/>
-    <tableColumn id="8" name="Migration rates" dataDxfId="1"/>
-    <tableColumn id="9" name="Total number of simulations" dataDxfId="0"/>
+    <tableColumn id="1" name="Drift scenario" dataDxfId="11"/>
+    <tableColumn id="2" name="Mechanisms explored" dataDxfId="10"/>
+    <tableColumn id="3" name="Colonization" dataDxfId="9"/>
+    <tableColumn id="4" name="Drift controlled by" dataDxfId="8"/>
+    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="7"/>
+    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="6"/>
+    <tableColumn id="7" name="Selection coefficient" dataDxfId="5"/>
+    <tableColumn id="8" name="Migration rates" dataDxfId="4"/>
+    <tableColumn id="9" name="Total number of simulations" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1696,14 +1872,14 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1714,140 +1890,143 @@
         <v>6</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="18"/>
+        <v>15</v>
+      </c>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="C8" s="39"/>
     </row>
     <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="18"/>
+        <v>69</v>
+      </c>
+      <c r="C11" s="39"/>
     </row>
     <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="C13" s="39"/>
+    </row>
+    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="C14" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1856,7 +2035,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1866,7 +2045,7 @@
     <col min="3" max="3" width="15.6640625" style="19" customWidth="1"/>
     <col min="4" max="4" width="20.5" style="19" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="19" customWidth="1"/>
     <col min="7" max="7" width="20" style="19" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" style="19" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" style="19" customWidth="1"/>
@@ -1874,31 +2053,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="49" thickTop="1" x14ac:dyDescent="0.2">
@@ -1906,31 +2085,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="I2" s="35">
         <v>12</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -1938,224 +2117,224 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I3" s="24">
         <v>30</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I4" s="24">
         <v>27</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I5" s="24">
         <f>27*3</f>
         <v>81</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I6" s="28">
         <v>30</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I7" s="28">
         <v>27</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
-        <v>7</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>67</v>
-      </c>
       <c r="F8" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I8" s="31">
         <v>9</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A9" s="29">
-        <v>8</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I9" s="31">
         <v>27</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating to reflect finished/running simulations
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31920" yWindow="3260" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HCN-by-Alleles" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Re-run</t>
   </si>
   <si>
     <t>Not done</t>
@@ -944,15 +941,6 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1317,6 +1305,15 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1494,16 +1491,16 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Parameter" dataDxfId="2"/>
-    <tableColumn id="2" name="Description" dataDxfId="1"/>
-    <tableColumn id="3" name="Mechanism controlled" dataDxfId="0"/>
+    <tableColumn id="1" name="Parameter" dataDxfId="16"/>
+    <tableColumn id="2" name="Description" dataDxfId="15"/>
+    <tableColumn id="3" name="Mechanism controlled" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:I9">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1516,15 +1513,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Drift scenario" dataDxfId="11"/>
-    <tableColumn id="2" name="Mechanisms explored" dataDxfId="10"/>
-    <tableColumn id="3" name="Colonization" dataDxfId="9"/>
-    <tableColumn id="4" name="Drift controlled by" dataDxfId="8"/>
-    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="7"/>
-    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="6"/>
-    <tableColumn id="7" name="Selection coefficient" dataDxfId="5"/>
-    <tableColumn id="8" name="Migration rates" dataDxfId="4"/>
-    <tableColumn id="9" name="Total number of simulations" dataDxfId="3"/>
+    <tableColumn id="1" name="Drift scenario" dataDxfId="8"/>
+    <tableColumn id="2" name="Mechanisms explored" dataDxfId="7"/>
+    <tableColumn id="3" name="Colonization" dataDxfId="6"/>
+    <tableColumn id="4" name="Drift controlled by" dataDxfId="5"/>
+    <tableColumn id="5" name="Parameters controlling drift" dataDxfId="4"/>
+    <tableColumn id="6" name="Initial allele frequencies" dataDxfId="3"/>
+    <tableColumn id="7" name="Selection coefficient" dataDxfId="2"/>
+    <tableColumn id="8" name="Migration rates" dataDxfId="1"/>
+    <tableColumn id="9" name="Total number of simulations" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1895,10 +1892,10 @@
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>20</v>
@@ -1906,24 +1903,24 @@
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1952,7 +1949,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -1960,7 +1957,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="39"/>
     </row>
@@ -1969,7 +1966,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>21</v>
@@ -1977,19 +1974,19 @@
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="39"/>
     </row>
@@ -2015,10 +2012,10 @@
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>67</v>
       </c>
       <c r="C14" s="39"/>
     </row>
@@ -2035,7 +2032,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2053,7 +2050,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>38</v>
@@ -2091,7 +2088,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>32</v>
@@ -2126,7 +2123,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>36</v>
@@ -2155,13 +2152,13 @@
         <v>33</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>33</v>
@@ -2190,10 +2187,10 @@
         <v>31</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>33</v>
@@ -2206,7 +2203,7 @@
         <v>81</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2217,7 +2214,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>33</v>
@@ -2238,7 +2235,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -2255,13 +2252,13 @@
         <v>31</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="22" t="s">
         <v>28</v>
@@ -2270,12 +2267,12 @@
         <v>27</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>43</v>
@@ -2284,16 +2281,16 @@
         <v>33</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>28</v>
@@ -2302,30 +2299,30 @@
         <v>9</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>28</v>
@@ -2334,7 +2331,7 @@
         <v>27</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated table with new simulations varying the minimum carrying capacity
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Not done</t>
-  </si>
-  <si>
-    <t>Max K = 1000 (Urban); Min K = 10 (Rural)</t>
   </si>
   <si>
     <t>Spatial gradient in K from Rural to Urban</t>
@@ -425,6 +422,58 @@
   </si>
   <si>
     <t>Drift scenario</t>
+  </si>
+  <si>
+    <r>
+      <t>Minimum carrying capacity (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>): 10; 100; 500; 1000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Minimum carrying capacity (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>): 10</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -759,7 +808,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -789,8 +838,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -907,8 +960,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -923,6 +982,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -937,6 +998,8 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
@@ -1500,8 +1563,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I10" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1892,10 +1955,10 @@
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>20</v>
@@ -1903,24 +1966,24 @@
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1949,7 +2012,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -1957,7 +2020,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="39"/>
     </row>
@@ -1966,7 +2029,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>21</v>
@@ -1974,19 +2037,19 @@
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="39"/>
     </row>
@@ -2012,10 +2075,10 @@
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>65</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>66</v>
       </c>
       <c r="C14" s="39"/>
     </row>
@@ -2029,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2050,7 +2113,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>38</v>
@@ -2077,7 +2140,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="49" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32">
         <v>1</v>
       </c>
@@ -2088,10 +2151,10 @@
         <v>33</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>36</v>
@@ -2100,65 +2163,65 @@
         <v>33</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="35">
         <v>12</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>44</v>
+      <c r="J2" s="41" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
-        <v>2</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="24">
-        <v>30</v>
+      <c r="H3" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="35">
+        <v>12</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>33</v>
@@ -2167,30 +2230,30 @@
         <v>28</v>
       </c>
       <c r="I4" s="24">
-        <v>27</v>
-      </c>
-      <c r="J4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>33</v>
@@ -2199,104 +2262,104 @@
         <v>28</v>
       </c>
       <c r="I5" s="24">
+        <v>27</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>2</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="24">
         <f>27*3</f>
         <v>81</v>
       </c>
-      <c r="J5" s="20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="J6" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="26">
         <v>1</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B7" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="C7" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E7" s="27" t="s">
         <v>42</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="28">
-        <v>30</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
-        <v>2</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>51</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="H7" s="22" t="s">
         <v>28</v>
       </c>
       <c r="I7" s="28">
+        <v>30</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="26">
+        <v>2</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="28">
         <v>27</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="31">
-        <v>9</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>45</v>
@@ -2304,33 +2367,65 @@
     </row>
     <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="31">
+        <v>9</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="31">
         <v>27</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J10" s="20" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated table with running simulations
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -350,9 +350,6 @@
     <t>2 (modified)</t>
   </si>
   <si>
-    <t>None.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -474,6 +471,9 @@
       </rPr>
       <t>): 10</t>
     </r>
+  </si>
+  <si>
+    <t>Not interesting</t>
   </si>
 </sst>
 </file>
@@ -2092,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2111,9 +2111,9 @@
     <col min="9" max="9" width="14.33203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>38</v>
@@ -2140,7 +2140,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32">
         <v>1</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>46</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>36</v>
@@ -2172,7 +2172,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="32">
         <v>1</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>46</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="33" t="s">
         <v>36</v>
@@ -2204,7 +2204,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>2</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>1</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>32</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>33</v>
@@ -2268,7 +2268,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>2</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>49</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>33</v>
@@ -2301,7 +2301,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>1</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>33</v>
@@ -2333,7 +2333,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
         <v>2</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>36</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>28</v>
@@ -2364,8 +2364,11 @@
       <c r="J8" s="20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>69</v>
       </c>
@@ -2379,25 +2382,25 @@
         <v>47</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="31">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>70</v>
       </c>
@@ -2417,13 +2420,13 @@
         <v>36</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="31">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Incorporated Rob's comments and finished results draft
</commit_message>
<xml_diff>
--- a/SEC_Manuscript-Tables.xlsx
+++ b/SEC_Manuscript-Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HCN-by-Alleles" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Number of rows</t>
-  </si>
-  <si>
-    <t>Number of columns</t>
-  </si>
-  <si>
     <t>Founder proportion</t>
   </si>
   <si>
@@ -73,12 +67,6 @@
     <t>Intrinsic rate of population increase</t>
   </si>
   <si>
-    <t>Number of rows on the landscape. Fixed at 1 since we are simulating a one-dimensional, linear matrix.</t>
-  </si>
-  <si>
-    <t>Number of columns on the landscape. Fixed at 40 since we are simulating 40 linearly distributed patches</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proportion of alleles sampled when founding a new populations. Lower proportions results in stronger effects of drift. </t>
   </si>
   <si>
@@ -86,18 +74,6 @@
   </si>
   <si>
     <t>Number of generations to run simulations once all patched on the landscape have been colonized with populations. Fixed at 500</t>
-  </si>
-  <si>
-    <t>Mechanism controlled</t>
-  </si>
-  <si>
-    <t>Gene flow</t>
-  </si>
-  <si>
-    <t>Selection</t>
-  </si>
-  <si>
-    <t>Within-population dynamics</t>
   </si>
   <si>
     <t>Drift controlled by</t>
@@ -259,12 +235,6 @@
     <t xml:space="preserve">Determines the carrying capacity of the smallest habitat patch on the landscape (rural-most or urban-most population). </t>
   </si>
   <si>
-    <t>Drift (scenario 2, see text)</t>
-  </si>
-  <si>
-    <t>Drift (scenario 1, see text)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maximum strength of selection acting on cyanogenic or acyanogenic genotypes. Actual strength of selection depends on a population's position in the landscape matrix. </t>
   </si>
   <si>
@@ -474,13 +444,86 @@
   </si>
   <si>
     <t>Not interesting</t>
+  </si>
+  <si>
+    <r>
+      <t>Li–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ý</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Li</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CYP79D15–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ý</t>
+    </r>
+  </si>
+  <si>
+    <t>Ý</t>
+  </si>
+  <si>
+    <t>ß</t>
+  </si>
+  <si>
+    <r>
+      <t>CYP79D15–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -555,6 +598,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -571,7 +629,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,7 +866,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -842,8 +900,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -895,9 +961,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,17 +1020,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -984,6 +1065,10 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1000,9 +1085,13 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1370,9 +1459,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1531,32 +1617,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="A1:C5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="CYP79D15" dataDxfId="19"/>
-    <tableColumn id="2" name="Li" dataDxfId="18"/>
-    <tableColumn id="3" name="HCN" dataDxfId="17"/>
+    <tableColumn id="1" name="CYP79D15" dataDxfId="18"/>
+    <tableColumn id="2" name="Li" dataDxfId="17"/>
+    <tableColumn id="3" name="HCN" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C14" totalsRowShown="0">
-  <autoFilter ref="A1:C14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Parameter" dataDxfId="16"/>
-    <tableColumn id="2" name="Description" dataDxfId="15"/>
-    <tableColumn id="3" name="Mechanism controlled" dataDxfId="14"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Parameter" dataDxfId="15"/>
+    <tableColumn id="2" name="Description" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1853,18 +1937,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection activeCell="G3" sqref="E1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1874,8 +1959,15 @@
       <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="40"/>
+      <c r="F1" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1885,8 +1977,17 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1896,8 +1997,17 @@
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1908,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1929,158 +2039,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="39"/>
-    </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="39"/>
-    </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="39"/>
-    </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="39"/>
-    </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>60</v>
-      </c>
       <c r="B11" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="39"/>
-    </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="39"/>
-    </row>
-    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="39"/>
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2094,342 +2159,342 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="19"/>
-    <col min="2" max="2" width="21.83203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="19" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="20" style="19" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="18"/>
+    <col min="2" max="2" width="21.83203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="18" customWidth="1"/>
+    <col min="7" max="7" width="20" style="18" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="E2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="34">
+        <v>12</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="31">
+        <v>1</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="34">
+        <v>12</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="23">
+        <v>30</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
+        <v>1</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="F5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32">
-        <v>1</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="33" t="s">
+      <c r="H5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="23">
+        <v>27</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="35">
-        <v>12</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="32">
-        <v>1</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="35">
-        <v>12</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
+    </row>
+    <row r="6" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="24">
-        <v>30</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
-        <v>1</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="24">
-        <v>27</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
-        <v>2</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="24">
+      <c r="C6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="23">
         <f>27*3</f>
         <v>81</v>
       </c>
-      <c r="J6" s="20" t="s">
-        <v>45</v>
+      <c r="J6" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
+      <c r="A7" s="25">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="27">
+        <v>30</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>2</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="27" t="s">
+      <c r="F8" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="27">
+        <v>27</v>
+      </c>
+      <c r="J8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="K8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="28">
+      <c r="G9" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="30">
         <v>30</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J9" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
-        <v>2</v>
-      </c>
-      <c r="B8" s="27" t="s">
+    <row r="10" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="22" t="s">
+      <c r="D10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="28">
-        <v>27</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="G10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="30">
+        <v>90</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="31">
-        <v>30</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="31">
-        <v>90</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>